<commit_message>
Worked on produciton files ... rearranged a directories a bit.
</commit_message>
<xml_diff>
--- a/fixed/white/CPL_JLCPCB_white.xlsx
+++ b/fixed/white/CPL_JLCPCB_white.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -37,19 +37,49 @@
     <t xml:space="preserve">Rotation</t>
   </si>
   <si>
-    <t xml:space="preserve">D1   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   top </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1   </t>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
   </si>
 </sst>
 </file>
@@ -153,9 +183,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -166,134 +200,304 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="2" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="8.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>-53.665</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>60.33</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>-54.63</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>67.14</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>-53.65</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>63.15</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>-64.95</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>61.925</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>-64.955</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="n">
         <v>62.7</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>-60</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="n">
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="n">
         <v>52.78</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>-60</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="n">
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="n">
         <v>72.62</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>-60</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="n">
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>58.55</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>-64.1625</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>68.87</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>-63.05</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>65.965</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>-66.975</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>68.88</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>-66.12</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>-54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="n">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>62.825</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>-54.74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>65.9625</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>-64.425</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4" t="n">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>